<commit_message>
Adjust available door styles to match only those listed in provided data
Modify the doorTypes arrays in app.js to reflect door types directly from the Excel data, removing derived logic.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 0646a5b4-ba54-4146-8119-cc31c948a5ea
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/873c23c0-c18f-4e09-9f8d-38c5cb319996/ca8586ce-aa4c-4018-adea-52c388c67cea.jpg
</commit_message>
<xml_diff>
--- a/attached_assets/Product Data.xlsx
+++ b/attached_assets/Product Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bathcraft-my.sharepoint.com/personal/olep00903843_maax_com/Documents/PythonScripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="11_8E13AE15F5EA82F19A54427495912BA654E97DEA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26977FBE-7947-4550-946F-39E60971CFE5}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="11_8E13AE15F5EA82F19A54427495912BA654E97DEA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C4F6BDD-0A2B-461A-90B5-689B75C2BB47}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-2640" windowWidth="38640" windowHeight="21120" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-2640" windowWidth="38640" windowHeight="21120" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shower Bases" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Bathtubs!$A$1:$M$237</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Enclosures!$A$1:$I$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Enclosures!$A$1:$K$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Return Panels'!$A$1:$F$33</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Screens!$A$1:$G$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Shower Doors'!$A$1:$N$219</definedName>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7038" uniqueCount="1764">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7062" uniqueCount="1764">
   <si>
     <t>Unique ID</t>
   </si>
@@ -21664,8 +21664,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:N219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N42" sqref="N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31216,10 +31216,10 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Sheet10"/>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31227,11 +31227,11 @@
     <col min="1" max="1" width="25.88671875" customWidth="1"/>
     <col min="2" max="2" width="34.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.77734375" customWidth="1"/>
-    <col min="4" max="9" width="25.88671875" customWidth="1"/>
-    <col min="12" max="12" width="61.6640625" customWidth="1"/>
+    <col min="4" max="11" width="25.88671875" customWidth="1"/>
+    <col min="14" max="14" width="61.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -31251,16 +31251,22 @@
         <v>1654</v>
       </c>
       <c r="G1" t="s">
+        <v>1761</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1757</v>
+      </c>
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1655</v>
       </c>
@@ -31280,16 +31286,22 @@
         <v>1657</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>1762</v>
       </c>
       <c r="H2" t="s">
+        <v>1760</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
         <v>325</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>1124</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1658</v>
       </c>
@@ -31309,16 +31321,22 @@
         <v>944</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>1762</v>
       </c>
       <c r="H3" t="s">
+        <v>1759</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
         <v>315</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>1152</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1660</v>
       </c>
@@ -31338,16 +31356,22 @@
         <v>1657</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>1762</v>
       </c>
       <c r="H4" t="s">
+        <v>1760</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
         <v>325</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>1124</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1662</v>
       </c>
@@ -31367,16 +31391,22 @@
         <v>1386</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>1762</v>
       </c>
       <c r="H5" t="s">
+        <v>1760</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
         <v>325</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>1124</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1664</v>
       </c>
@@ -31396,16 +31426,22 @@
         <v>1666</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
+        <v>1762</v>
       </c>
       <c r="H6" t="s">
-        <v>19</v>
+        <v>1760</v>
       </c>
       <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" t="s">
         <v>1205</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1667</v>
       </c>
@@ -31425,16 +31461,22 @@
         <v>1657</v>
       </c>
       <c r="G7" t="s">
-        <v>18</v>
+        <v>1762</v>
       </c>
       <c r="H7" t="s">
+        <v>1760</v>
+      </c>
+      <c r="I7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" t="s">
         <v>325</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>1124</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1669</v>
       </c>
@@ -31454,16 +31496,22 @@
         <v>1386</v>
       </c>
       <c r="G8" t="s">
-        <v>18</v>
+        <v>1762</v>
       </c>
       <c r="H8" t="s">
+        <v>1760</v>
+      </c>
+      <c r="I8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" t="s">
         <v>325</v>
       </c>
-      <c r="I8" t="s">
+      <c r="K8" t="s">
         <v>1124</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1671</v>
       </c>
@@ -31483,16 +31531,22 @@
         <v>1386</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
+        <v>1762</v>
       </c>
       <c r="H9" t="s">
+        <v>1760</v>
+      </c>
+      <c r="I9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" t="s">
         <v>325</v>
       </c>
-      <c r="I9" t="s">
+      <c r="K9" t="s">
         <v>1124</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1673</v>
       </c>
@@ -31512,16 +31566,22 @@
         <v>1666</v>
       </c>
       <c r="G10" t="s">
-        <v>18</v>
+        <v>1762</v>
       </c>
       <c r="H10" t="s">
-        <v>19</v>
+        <v>1760</v>
       </c>
       <c r="I10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" t="s">
         <v>1205</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1675</v>
       </c>
@@ -31541,16 +31601,22 @@
         <v>1657</v>
       </c>
       <c r="G11" t="s">
-        <v>18</v>
+        <v>1762</v>
       </c>
       <c r="H11" t="s">
+        <v>1760</v>
+      </c>
+      <c r="I11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" t="s">
         <v>325</v>
       </c>
-      <c r="I11" t="s">
+      <c r="K11" t="s">
         <v>1124</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1677</v>
       </c>
@@ -31570,17 +31636,23 @@
         <v>1386</v>
       </c>
       <c r="G12" t="s">
-        <v>18</v>
+        <v>1762</v>
       </c>
       <c r="H12" t="s">
+        <v>1760</v>
+      </c>
+      <c r="I12" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" t="s">
         <v>325</v>
       </c>
-      <c r="I12" t="s">
+      <c r="K12" t="s">
         <v>1124</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I14" xr:uid="{00000000-0009-0000-0000-000008000000}"/>
+  <autoFilter ref="A1:K14" xr:uid="{00000000-0009-0000-0000-000008000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update product information to include more enclosure specifications
Update Product Data.xlsx files in attached_assets and data to reflect schema changes.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 0646a5b4-ba54-4146-8119-cc31c948a5ea
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/873c23c0-c18f-4e09-9f8d-38c5cb319996/9f9e6a8a-888d-466f-b8a8-9cbb080d3543.jpg
</commit_message>
<xml_diff>
--- a/attached_assets/Product Data.xlsx
+++ b/attached_assets/Product Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bathcraft-my.sharepoint.com/personal/olep00903843_maax_com/Documents/PythonScripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="50" documentId="11_8E13AE15F5EA82F19A54427495912BA654E97DEA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26977FBE-7947-4550-946F-39E60971CFE5}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="11_8E13AE15F5EA82F19A54427495912BA654E97DEA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1C4F6BDD-0A2B-461A-90B5-689B75C2BB47}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-2640" windowWidth="38640" windowHeight="21120" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-2640" windowWidth="38640" windowHeight="21120" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Shower Bases" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Bathtubs!$A$1:$M$237</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Enclosures!$A$1:$I$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Enclosures!$A$1:$K$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Return Panels'!$A$1:$F$33</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Screens!$A$1:$G$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Shower Doors'!$A$1:$N$219</definedName>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7038" uniqueCount="1764">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7062" uniqueCount="1764">
   <si>
     <t>Unique ID</t>
   </si>
@@ -21664,8 +21664,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:N219"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N42" sqref="N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31216,10 +31216,10 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Sheet10"/>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31227,11 +31227,11 @@
     <col min="1" max="1" width="25.88671875" customWidth="1"/>
     <col min="2" max="2" width="34.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="34.77734375" customWidth="1"/>
-    <col min="4" max="9" width="25.88671875" customWidth="1"/>
-    <col min="12" max="12" width="61.6640625" customWidth="1"/>
+    <col min="4" max="11" width="25.88671875" customWidth="1"/>
+    <col min="14" max="14" width="61.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -31251,16 +31251,22 @@
         <v>1654</v>
       </c>
       <c r="G1" t="s">
+        <v>1761</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1757</v>
+      </c>
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1655</v>
       </c>
@@ -31280,16 +31286,22 @@
         <v>1657</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>1762</v>
       </c>
       <c r="H2" t="s">
+        <v>1760</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
         <v>325</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>1124</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1658</v>
       </c>
@@ -31309,16 +31321,22 @@
         <v>944</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>1762</v>
       </c>
       <c r="H3" t="s">
+        <v>1759</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
         <v>315</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>1152</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1660</v>
       </c>
@@ -31338,16 +31356,22 @@
         <v>1657</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>1762</v>
       </c>
       <c r="H4" t="s">
+        <v>1760</v>
+      </c>
+      <c r="I4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" t="s">
         <v>325</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>1124</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1662</v>
       </c>
@@ -31367,16 +31391,22 @@
         <v>1386</v>
       </c>
       <c r="G5" t="s">
-        <v>18</v>
+        <v>1762</v>
       </c>
       <c r="H5" t="s">
+        <v>1760</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
         <v>325</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>1124</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1664</v>
       </c>
@@ -31396,16 +31426,22 @@
         <v>1666</v>
       </c>
       <c r="G6" t="s">
-        <v>18</v>
+        <v>1762</v>
       </c>
       <c r="H6" t="s">
-        <v>19</v>
+        <v>1760</v>
       </c>
       <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" t="s">
         <v>1205</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1667</v>
       </c>
@@ -31425,16 +31461,22 @@
         <v>1657</v>
       </c>
       <c r="G7" t="s">
-        <v>18</v>
+        <v>1762</v>
       </c>
       <c r="H7" t="s">
+        <v>1760</v>
+      </c>
+      <c r="I7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" t="s">
         <v>325</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>1124</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1669</v>
       </c>
@@ -31454,16 +31496,22 @@
         <v>1386</v>
       </c>
       <c r="G8" t="s">
-        <v>18</v>
+        <v>1762</v>
       </c>
       <c r="H8" t="s">
+        <v>1760</v>
+      </c>
+      <c r="I8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" t="s">
         <v>325</v>
       </c>
-      <c r="I8" t="s">
+      <c r="K8" t="s">
         <v>1124</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1671</v>
       </c>
@@ -31483,16 +31531,22 @@
         <v>1386</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
+        <v>1762</v>
       </c>
       <c r="H9" t="s">
+        <v>1760</v>
+      </c>
+      <c r="I9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" t="s">
         <v>325</v>
       </c>
-      <c r="I9" t="s">
+      <c r="K9" t="s">
         <v>1124</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1673</v>
       </c>
@@ -31512,16 +31566,22 @@
         <v>1666</v>
       </c>
       <c r="G10" t="s">
-        <v>18</v>
+        <v>1762</v>
       </c>
       <c r="H10" t="s">
-        <v>19</v>
+        <v>1760</v>
       </c>
       <c r="I10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" t="s">
         <v>1205</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1675</v>
       </c>
@@ -31541,16 +31601,22 @@
         <v>1657</v>
       </c>
       <c r="G11" t="s">
-        <v>18</v>
+        <v>1762</v>
       </c>
       <c r="H11" t="s">
+        <v>1760</v>
+      </c>
+      <c r="I11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" t="s">
         <v>325</v>
       </c>
-      <c r="I11" t="s">
+      <c r="K11" t="s">
         <v>1124</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1677</v>
       </c>
@@ -31570,17 +31636,23 @@
         <v>1386</v>
       </c>
       <c r="G12" t="s">
-        <v>18</v>
+        <v>1762</v>
       </c>
       <c r="H12" t="s">
+        <v>1760</v>
+      </c>
+      <c r="I12" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" t="s">
         <v>325</v>
       </c>
-      <c r="I12" t="s">
+      <c r="K12" t="s">
         <v>1124</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I14" xr:uid="{00000000-0009-0000-0000-000008000000}"/>
+  <autoFilter ref="A1:K14" xr:uid="{00000000-0009-0000-0000-000008000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>